<commit_message>
not(mat); 0-no 1-yes update
</commit_message>
<xml_diff>
--- a/mat/ferries_wheels.xlsx
+++ b/mat/ferries_wheels.xlsx
@@ -1,133 +1,960 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView windowWidth="28695" windowHeight="13155" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+  <borders count="9">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="303030"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:CL90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R20" activeCellId="0" sqref="R20"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col min="1" max="1025" width="11.5166666666667"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:90">
       <c r="A1" s="1" t="b">
         <v>0</v>
       </c>
@@ -399,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:90">
       <c r="A2" s="1" t="b">
         <v>0</v>
       </c>
@@ -671,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:90">
       <c r="A3" s="1" t="b">
         <v>0</v>
       </c>
@@ -943,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:90">
       <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
@@ -1215,7 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:90">
       <c r="A5" s="1" t="b">
         <v>0</v>
       </c>
@@ -1487,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:90">
       <c r="A6" s="1" t="b">
         <v>0</v>
       </c>
@@ -1759,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:90">
       <c r="A7" s="1" t="b">
         <v>0</v>
       </c>
@@ -2031,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:90">
       <c r="A8" s="1" t="b">
         <v>0</v>
       </c>
@@ -2303,7 +3130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:90">
       <c r="A9" s="1" t="b">
         <v>0</v>
       </c>
@@ -2575,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:90">
       <c r="A10" s="1" t="b">
         <v>0</v>
       </c>
@@ -2847,7 +3674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:90">
       <c r="A11" s="1" t="b">
         <v>0</v>
       </c>
@@ -3119,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:90">
       <c r="A12" s="1" t="b">
         <v>0</v>
       </c>
@@ -3391,7 +4218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:90">
       <c r="A13" s="1" t="b">
         <v>0</v>
       </c>
@@ -3663,7 +4490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:90">
       <c r="A14" s="1" t="b">
         <v>0</v>
       </c>
@@ -3935,7 +4762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:90">
       <c r="A15" s="1" t="b">
         <v>0</v>
       </c>
@@ -4207,7 +5034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:90">
       <c r="A16" s="1" t="b">
         <v>0</v>
       </c>
@@ -4479,7 +5306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:90">
       <c r="A17" s="1" t="b">
         <v>0</v>
       </c>
@@ -4751,7 +5578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:90">
       <c r="A18" s="1" t="b">
         <v>0</v>
       </c>
@@ -5023,7 +5850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:90">
       <c r="A19" s="1" t="b">
         <v>0</v>
       </c>
@@ -5295,7 +6122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:90">
       <c r="A20" s="1" t="b">
         <v>0</v>
       </c>
@@ -5567,7 +6394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:90">
       <c r="A21" s="1" t="b">
         <v>0</v>
       </c>
@@ -5839,7 +6666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:90">
       <c r="A22" s="1" t="b">
         <v>0</v>
       </c>
@@ -6111,7 +6938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:90">
       <c r="A23" s="1" t="b">
         <v>0</v>
       </c>
@@ -6383,7 +7210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:90">
       <c r="A24" s="1" t="b">
         <v>0</v>
       </c>
@@ -6655,7 +7482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:90">
       <c r="A25" s="1" t="b">
         <v>0</v>
       </c>
@@ -6927,7 +7754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:90">
       <c r="A26" s="1" t="b">
         <v>0</v>
       </c>
@@ -7199,7 +8026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:90">
       <c r="A27" s="1" t="b">
         <v>0</v>
       </c>
@@ -7471,7 +8298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:90">
       <c r="A28" s="1" t="b">
         <v>0</v>
       </c>
@@ -7743,7 +8570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:90">
       <c r="A29" s="1" t="b">
         <v>0</v>
       </c>
@@ -8015,7 +8842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:90">
       <c r="A30" s="1" t="b">
         <v>0</v>
       </c>
@@ -8287,7 +9114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:90">
       <c r="A31" s="1" t="b">
         <v>0</v>
       </c>
@@ -8559,7 +9386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:90">
       <c r="A32" s="1" t="b">
         <v>0</v>
       </c>
@@ -8831,7 +9658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:90">
       <c r="A33" s="1" t="b">
         <v>0</v>
       </c>
@@ -9103,7 +9930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:90">
       <c r="A34" s="1" t="b">
         <v>0</v>
       </c>
@@ -9375,7 +10202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:90">
       <c r="A35" s="1" t="b">
         <v>0</v>
       </c>
@@ -9647,7 +10474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:90">
       <c r="A36" s="1" t="b">
         <v>0</v>
       </c>
@@ -9919,7 +10746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:90">
       <c r="A37" s="1" t="b">
         <v>0</v>
       </c>
@@ -10191,7 +11018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:90">
       <c r="A38" s="1" t="b">
         <v>0</v>
       </c>
@@ -10463,7 +11290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:90">
       <c r="A39" s="1" t="b">
         <v>0</v>
       </c>
@@ -10735,7 +11562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:90">
       <c r="A40" s="1" t="b">
         <v>0</v>
       </c>
@@ -11007,7 +11834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:90">
       <c r="A41" s="1" t="b">
         <v>0</v>
       </c>
@@ -11279,7 +12106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:90">
       <c r="A42" s="1" t="b">
         <v>0</v>
       </c>
@@ -11551,7 +12378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:90">
       <c r="A43" s="1" t="b">
         <v>0</v>
       </c>
@@ -11823,7 +12650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:90">
       <c r="A44" s="1" t="b">
         <v>0</v>
       </c>
@@ -12095,7 +12922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:90">
       <c r="A45" s="1" t="b">
         <v>0</v>
       </c>
@@ -12367,7 +13194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:90">
       <c r="A46" s="1" t="b">
         <v>0</v>
       </c>
@@ -12639,7 +13466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:90">
       <c r="A47" s="1" t="b">
         <v>0</v>
       </c>
@@ -12911,7 +13738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:90">
       <c r="A48" s="1" t="b">
         <v>0</v>
       </c>
@@ -13183,7 +14010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:90">
       <c r="A49" s="1" t="b">
         <v>0</v>
       </c>
@@ -13455,7 +14282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:90">
       <c r="A50" s="1" t="b">
         <v>0</v>
       </c>
@@ -13727,7 +14554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:90">
       <c r="A51" s="1" t="b">
         <v>0</v>
       </c>
@@ -13999,7 +14826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:90">
       <c r="A52" s="1" t="b">
         <v>0</v>
       </c>
@@ -14271,7 +15098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:90">
       <c r="A53" s="1" t="b">
         <v>0</v>
       </c>
@@ -14543,7 +15370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:90">
       <c r="A54" s="1" t="b">
         <v>0</v>
       </c>
@@ -14815,7 +15642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:90">
       <c r="A55" s="1" t="b">
         <v>0</v>
       </c>
@@ -15087,7 +15914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:90">
       <c r="A56" s="1" t="b">
         <v>0</v>
       </c>
@@ -15359,7 +16186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:90">
       <c r="A57" s="1" t="b">
         <v>0</v>
       </c>
@@ -15631,7 +16458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:90">
       <c r="A58" s="1" t="b">
         <v>0</v>
       </c>
@@ -15903,7 +16730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:90">
       <c r="A59" s="1" t="b">
         <v>0</v>
       </c>
@@ -16175,7 +17002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:90">
       <c r="A60" s="1" t="b">
         <v>0</v>
       </c>
@@ -16447,7 +17274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:90">
       <c r="A61" s="1" t="b">
         <v>0</v>
       </c>
@@ -16719,7 +17546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:90">
       <c r="A62" s="1" t="b">
         <v>0</v>
       </c>
@@ -16991,7 +17818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:90">
       <c r="A63" s="1" t="b">
         <v>0</v>
       </c>
@@ -17263,7 +18090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:90">
       <c r="A64" s="1" t="b">
         <v>0</v>
       </c>
@@ -17535,7 +18362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:90">
       <c r="A65" s="1" t="b">
         <v>0</v>
       </c>
@@ -17807,7 +18634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:90">
       <c r="A66" s="1" t="b">
         <v>0</v>
       </c>
@@ -18079,7 +18906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:90">
       <c r="A67" s="1" t="b">
         <v>0</v>
       </c>
@@ -18351,7 +19178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:90">
       <c r="A68" s="1" t="b">
         <v>0</v>
       </c>
@@ -18623,7 +19450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:90">
       <c r="A69" s="1" t="b">
         <v>0</v>
       </c>
@@ -18895,7 +19722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:90">
       <c r="A70" s="1" t="b">
         <v>0</v>
       </c>
@@ -19167,7 +19994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:90">
       <c r="A71" s="1" t="b">
         <v>0</v>
       </c>
@@ -19439,7 +20266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:90">
       <c r="A72" s="1" t="b">
         <v>0</v>
       </c>
@@ -19711,7 +20538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:90">
       <c r="A73" s="1" t="b">
         <v>0</v>
       </c>
@@ -19983,7 +20810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:90">
       <c r="A74" s="1" t="b">
         <v>0</v>
       </c>
@@ -20255,7 +21082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:90">
       <c r="A75" s="1" t="b">
         <v>0</v>
       </c>
@@ -20527,7 +21354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:90">
       <c r="A76" s="1" t="b">
         <v>0</v>
       </c>
@@ -20799,7 +21626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:90">
       <c r="A77" s="1" t="b">
         <v>0</v>
       </c>
@@ -21071,7 +21898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:90">
       <c r="A78" s="1" t="b">
         <v>0</v>
       </c>
@@ -21343,7 +22170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:90">
       <c r="A79" s="1" t="b">
         <v>0</v>
       </c>
@@ -21615,7 +22442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:90">
       <c r="A80" s="1" t="b">
         <v>0</v>
       </c>
@@ -21887,7 +22714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:90">
       <c r="A81" s="1" t="b">
         <v>0</v>
       </c>
@@ -22159,7 +22986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:90">
       <c r="A82" s="1" t="b">
         <v>0</v>
       </c>
@@ -22431,7 +23258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:90">
       <c r="A83" s="1" t="b">
         <v>0</v>
       </c>
@@ -22703,7 +23530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:90">
       <c r="A84" s="1" t="b">
         <v>0</v>
       </c>
@@ -22975,7 +23802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:90">
       <c r="A85" s="1" t="b">
         <v>0</v>
       </c>
@@ -23247,7 +24074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:90">
       <c r="A86" s="1" t="b">
         <v>0</v>
       </c>
@@ -23519,7 +24346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:90">
       <c r="A87" s="1" t="b">
         <v>0</v>
       </c>
@@ -23791,7 +24618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:90">
       <c r="A88" s="1" t="b">
         <v>0</v>
       </c>
@@ -24063,7 +24890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:90">
       <c r="A89" s="1" t="b">
         <v>0</v>
       </c>
@@ -24335,7 +25162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:90">
       <c r="A90" s="1" t="b">
         <v>0</v>
       </c>
@@ -24608,10 +25435,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.02430555555556" bottom="1.02430555555556" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>